<commit_message>
Update Imppor Data PD
</commit_message>
<xml_diff>
--- a/excel/import-data-utama_pd.xlsx
+++ b/excel/import-data-utama_pd.xlsx
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>JENIS KELAMIN</t>
   </si>
@@ -500,6 +500,15 @@
   </si>
   <si>
     <t>3205106707020008</t>
+  </si>
+  <si>
+    <t>001456794</t>
+  </si>
+  <si>
+    <t>UDIN</t>
+  </si>
+  <si>
+    <t>3205106707020009</t>
   </si>
 </sst>
 </file>
@@ -930,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -1099,12 +1108,59 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <v>171814309</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5">
+        <v>37063</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
       <formula1>"Laki-laki,Perempuan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>"Islam,Kristen,Khatolik,Hindu,Budha"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>